<commit_message>
NMR fast exchange script interface - roughly done
</commit_message>
<xml_diff>
--- a/input/nmr/dsn.1/data.input.xlsx
+++ b/input/nmr/dsn.1/data.input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\nmr\dsn.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B042926-390D-430B-B223-1231FCCCAE94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360EF049-F1FF-437B-90E6-7660A51D4A92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stoich_coefficients" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,16 @@
     <sheet name="targets" sheetId="5" r:id="rId5"/>
     <sheet name="individual_shifts" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -443,7 +449,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,12 +464,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3.31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3.11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -770,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +906,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>8.3021999999999991</v>
+        <v>8.4596999999999998</v>
       </c>
       <c r="E2">
         <v>8.5451999999999995</v>
@@ -1144,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1172,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>8.3019999999999996</v>
+        <v>8.4596999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>